<commit_message>
fix template classroom save
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/classroomRegister.xlsx
+++ b/src/main/resources/excel/classroomRegister.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lms-platform-backend\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lms-platform-backend-master\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DC8029-EC9F-4A82-BEB0-11875D2AFA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B336F4-1899-4D8E-B619-E4B7B1BC0F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4856B4E8-8820-40DE-A7E0-F4C13E70EAD1}"/>
   </bookViews>
@@ -327,15 +327,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -348,6 +339,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,30 +682,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE08A3B-8ECF-4DE3-B3AF-8785E326BC43}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="14"/>
-    <col min="2" max="2" width="40.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="53" style="9" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="37" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="40.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="53" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="37" style="8" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -716,277 +717,277 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -996,6 +997,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0854B86D-C361-4531-9054-8790A5E0006E}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1012,14 +1014,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="13"/>
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>